<commit_message>
Added default taxonomy for UiPath public endpoint's ML models (Incoices, Purchase Orders, Receipts, Utility Bills)
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/masaki_kumamoto_uipath_com/Documents/Documents/UiPath/04_Templates/DocumentUnderstandingEvaluationTemplate/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\masaki.kumamoto\OneDrive - UiPath\Documents\UiPath\04_Templates\DocumentUnderstandingEvaluationTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FD44D52C-1D66-4EE7-B865-7908FF23D67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A9BAC94-9201-45D2-A363-F64FE54E4482}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4E033E-2F83-49A7-8D7F-19673455E8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="-18300" windowWidth="28800" windowHeight="15885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSettings" sheetId="14" r:id="rId1"/>
@@ -2251,7 +2251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BCE469-BC90-4982-9CD3-7942BA4D4066}">
   <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
@@ -2808,7 +2808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E20320B-E7C7-4ECD-A0DB-4C2AE6EF68EB}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
- Include ExtractedPage and ActualPAge in the reports - Include timestamp as a strorage bucket folder name - Not to  create a new Excel file when AL_UseExistingActionListExcel is True
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/masaki_kumamoto_uipath_com/Documents/Documents/UiPath/04_Templates/DocumentUnderstandingEvaluationTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4E033E-2F83-49A7-8D7F-19673455E8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9B4E033E-2F83-49A7-8D7F-19673455E8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C426517C-D6A4-4D26-A92C-A6E0B5F3FE0A}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicSettings" sheetId="14" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>AC_AssignUserEmail</t>
   </si>
   <si>
-    <t>SB_BacketName</t>
-  </si>
-  <si>
     <t>DU_IntelligentFromExtractor_Endpoint</t>
   </si>
   <si>
@@ -442,9 +439,6 @@
   <si>
     <t>[Assign Tasks] - TaskUserAssignments
 https://docs.uipath.com/activities/lang-en/docs/assign-tasks</t>
-  </si>
-  <si>
-    <t>Finance/AccountsPayable</t>
   </si>
   <si>
     <t>[Create Document Validation Action] - BucketDirectoryPath
@@ -581,6 +575,12 @@
     <t>Document Type Id which [Data Extraction Scope] Activity uses.
 You can find the value in Taxonomy Manager once you create a taxonomy.
 If you use Classification activity, you do NOT need to specify this field.</t>
+  </si>
+  <si>
+    <t>SB_BucketName</t>
+  </si>
+  <si>
+    <t>Finance\AccountsPayable</t>
   </si>
 </sst>
 </file>
@@ -2274,16 +2274,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="29" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G1" s="29" t="s">
         <v>28</v>
@@ -2313,70 +2313,70 @@
     </row>
     <row r="2" spans="1:29" s="43" customFormat="1" ht="60">
       <c r="A2" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="43" customFormat="1" ht="75">
       <c r="A3" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F3" s="33"/>
       <c r="G3" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="75">
       <c r="A4" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="120">
       <c r="A5" s="30" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B5" s="31" t="b">
         <v>0</v>
@@ -2385,27 +2385,27 @@
         <v>0</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:29" ht="90">
       <c r="A6" s="39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
@@ -2446,7 +2446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7BE991-0805-438E-A28D-2AC2A75CC1EB}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
@@ -2469,16 +2469,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="29" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G1" s="29" t="s">
         <v>28</v>
@@ -2512,16 +2512,16 @@
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="33" t="s">
         <v>111</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>112</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>32</v>
@@ -2554,16 +2554,16 @@
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" s="33" t="s">
         <v>32</v>
@@ -2592,22 +2592,22 @@
     </row>
     <row r="4" spans="1:29" ht="240">
       <c r="A4" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="33" t="s">
         <v>32</v>
@@ -2636,7 +2636,7 @@
     </row>
     <row r="5" spans="1:29" ht="120">
       <c r="A5" s="30" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B5" s="45">
         <v>0.99980000000000002</v>
@@ -2645,10 +2645,10 @@
         <v>0.99980000000000002</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33" t="s">
@@ -2657,7 +2657,7 @@
     </row>
     <row r="6" spans="1:29" ht="120">
       <c r="A6" s="30" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B6" s="45">
         <v>0.95989999999999998</v>
@@ -2666,10 +2666,10 @@
         <v>0.95</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F6" s="33"/>
       <c r="G6" s="33" t="s">
@@ -2678,22 +2678,22 @@
     </row>
     <row r="7" spans="1:29" ht="150">
       <c r="A7" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G7" s="33" t="s">
         <v>32</v>
@@ -2701,22 +2701,22 @@
     </row>
     <row r="8" spans="1:29" ht="165">
       <c r="A8" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="33" t="s">
         <v>137</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>139</v>
       </c>
       <c r="G8" s="33" t="s">
         <v>32</v>
@@ -2724,22 +2724,22 @@
     </row>
     <row r="9" spans="1:29" ht="165">
       <c r="A9" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="33" t="s">
         <v>32</v>
@@ -2747,22 +2747,22 @@
     </row>
     <row r="10" spans="1:29" ht="165">
       <c r="A10" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F10" s="33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>32</v>
@@ -2830,16 +2830,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>28</v>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="2" spans="1:29" ht="30">
       <c r="A2" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="31" t="b">
         <v>1</v>
@@ -2878,10 +2878,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F2" s="37"/>
       <c r="G2" s="36" t="s">
@@ -2894,16 +2894,16 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G3" s="36" t="s">
         <v>31</v>
@@ -2914,19 +2914,19 @@
         <v>34</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C4" s="50" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G4" s="50" t="s">
         <v>31</v>
@@ -2937,19 +2937,19 @@
         <v>26</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G5" s="36" t="s">
         <v>30</v>
@@ -2957,22 +2957,22 @@
     </row>
     <row r="6" spans="1:29" ht="165">
       <c r="A6" s="34" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G6" s="36" t="s">
         <v>29</v>
@@ -2984,16 +2984,16 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="50" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="D7" s="50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="50" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G7" s="50" t="s">
         <v>29</v>
@@ -3062,10 +3062,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>3</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="2" spans="1:28" ht="30">
       <c r="A2" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="12" t="b">
         <v>0</v>
@@ -3107,51 +3107,51 @@
         <v>0</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:28">
       <c r="A3" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="60">
       <c r="A4" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -3164,7 +3164,7 @@
     </row>
     <row r="6" spans="1:28" ht="30">
       <c r="A6" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="12" t="b">
         <v>0</v>
@@ -3173,33 +3173,33 @@
         <v>0</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="75">
       <c r="A7" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:28">
@@ -3212,7 +3212,7 @@
     </row>
     <row r="9" spans="1:28" ht="90">
       <c r="A9" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="12" t="b">
         <v>0</v>
@@ -3221,33 +3221,33 @@
         <v>0</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="45">
       <c r="A10" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:28">
@@ -3260,7 +3260,7 @@
     </row>
     <row r="12" spans="1:28" ht="30">
       <c r="A12" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="12" t="b">
         <v>0</v>
@@ -3269,87 +3269,87 @@
         <v>0</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="45">
       <c r="A13" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:28">
       <c r="A14" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:28">
       <c r="A15" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:28">
       <c r="A16" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3362,7 +3362,7 @@
     </row>
     <row r="18" spans="1:6" ht="30">
       <c r="A18" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="12" t="b">
         <v>0</v>
@@ -3371,69 +3371,69 @@
         <v>0</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30">
       <c r="A19" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30">
       <c r="A20" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="45">
       <c r="A21" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3446,7 +3446,7 @@
     </row>
     <row r="23" spans="1:6" ht="30">
       <c r="A23" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" s="12" t="b">
         <v>0</v>
@@ -3455,33 +3455,33 @@
         <v>0</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30">
       <c r="A24" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3494,7 +3494,7 @@
     </row>
     <row r="26" spans="1:6" ht="30">
       <c r="A26" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="12" t="b">
         <v>0</v>
@@ -3503,51 +3503,51 @@
         <v>0</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30">
       <c r="A28" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3560,7 +3560,7 @@
     </row>
     <row r="30" spans="1:6" ht="30">
       <c r="A30" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="12" t="b">
         <v>0</v>
@@ -3569,33 +3569,33 @@
         <v>0</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="45">
       <c r="A31" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -3645,10 +3645,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>19</v>
@@ -3707,11 +3707,11 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>7</v>
@@ -3734,7 +3734,7 @@
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>23</v>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>12</v>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>20</v>
@@ -3782,7 +3782,7 @@
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>21</v>
@@ -3798,7 +3798,7 @@
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>22</v>
@@ -3807,19 +3807,19 @@
     </row>
     <row r="11" spans="1:28" ht="30">
       <c r="A11" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F11" s="27"/>
       <c r="G11" s="24"/>

</xml_diff>